<commit_message>
ChkPoint: a6_pd_model_estimation.py - initial commit
</commit_message>
<xml_diff>
--- a/data/list1_variables.xlsx
+++ b/data/list1_variables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\al_files\PycharmProjects\Python\CreditRiskModelingPython2022\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8402CBE4-3D84-4F1F-975B-1B746E331534}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{559F3A44-5AE8-41F7-BD7C-7CFD05981106}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2595" yWindow="930" windowWidth="24390" windowHeight="14010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PD_variables" sheetId="1" r:id="rId1"/>
@@ -33,19 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
-  <si>
-    <t>D</t>
-  </si>
-  <si>
-    <t>E</t>
-  </si>
-  <si>
-    <t>F</t>
-  </si>
-  <si>
-    <t>G</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="128">
   <si>
     <t>grade:A</t>
   </si>
@@ -68,18 +56,6 @@
     <t>grade:G</t>
   </si>
   <si>
-    <t>home_ownership:</t>
-  </si>
-  <si>
-    <t>RENT_OTHER_NONE_ANY</t>
-  </si>
-  <si>
-    <t>OWN</t>
-  </si>
-  <si>
-    <t>MORTGAGE</t>
-  </si>
-  <si>
     <t>home_ownership:RENT_OTHER_NONE_ANY</t>
   </si>
   <si>
@@ -93,6 +69,354 @@
   </si>
   <si>
     <t>Is Ref</t>
+  </si>
+  <si>
+    <t>addr_state:ND_NE_IA_NV_FL_HI_AL</t>
+  </si>
+  <si>
+    <t>addr_state:NM_VA</t>
+  </si>
+  <si>
+    <t>addr_state:NY</t>
+  </si>
+  <si>
+    <t>addr_state:OK_TN_MO_LA_MD_NC</t>
+  </si>
+  <si>
+    <t>addr_state:CA</t>
+  </si>
+  <si>
+    <t>addr_state:UT_KY_AZ_NJ</t>
+  </si>
+  <si>
+    <t>addr_state:AR_MI_PA_OH_MN</t>
+  </si>
+  <si>
+    <t>addr_state:RI_MA_DE_SD_IN</t>
+  </si>
+  <si>
+    <t>addr_state:GA_WA_OR</t>
+  </si>
+  <si>
+    <t>addr_state:WI_MT</t>
+  </si>
+  <si>
+    <t>addr_state:TX</t>
+  </si>
+  <si>
+    <t>addr_state:IL_CT</t>
+  </si>
+  <si>
+    <t>addr_state:KS_SC_CO_VT_AK_MS</t>
+  </si>
+  <si>
+    <t>addr_state:WV_NH_WY_DC_ME_ID</t>
+  </si>
+  <si>
+    <t>verification_status:Not Verified</t>
+  </si>
+  <si>
+    <t>verification_status:Source Verified</t>
+  </si>
+  <si>
+    <t>verification_status:Verified</t>
+  </si>
+  <si>
+    <t>purpose:educ__sm_b__wedd__ren_en__mov__house</t>
+  </si>
+  <si>
+    <t>purpose:credit_card</t>
+  </si>
+  <si>
+    <t>purpose:debt_consolidation</t>
+  </si>
+  <si>
+    <t>purpose:oth__med__vacation</t>
+  </si>
+  <si>
+    <t>purpose:major_purch__car__home_impr</t>
+  </si>
+  <si>
+    <t>initial_list_status:f</t>
+  </si>
+  <si>
+    <t>initial_list_status:w</t>
+  </si>
+  <si>
+    <t>term:36</t>
+  </si>
+  <si>
+    <t>term:60</t>
+  </si>
+  <si>
+    <t>emp_length:0</t>
+  </si>
+  <si>
+    <t>emp_length:1</t>
+  </si>
+  <si>
+    <t>emp_length:2-4</t>
+  </si>
+  <si>
+    <t>emp_length:5-6</t>
+  </si>
+  <si>
+    <t>emp_length:7-9</t>
+  </si>
+  <si>
+    <t>emp_length:10</t>
+  </si>
+  <si>
+    <t>mths_since_issue_d:&lt;38</t>
+  </si>
+  <si>
+    <t>mths_since_issue_d:38-39</t>
+  </si>
+  <si>
+    <t>mths_since_issue_d:40-41</t>
+  </si>
+  <si>
+    <t>mths_since_issue_d:42-48</t>
+  </si>
+  <si>
+    <t>mths_since_issue_d:49-52</t>
+  </si>
+  <si>
+    <t>mths_since_issue_d:53-64</t>
+  </si>
+  <si>
+    <t>mths_since_issue_d:65-84</t>
+  </si>
+  <si>
+    <t>mths_since_issue_d:&gt;84</t>
+  </si>
+  <si>
+    <t>int_rate:&lt;9.548</t>
+  </si>
+  <si>
+    <t>int_rate:9.548-12.025</t>
+  </si>
+  <si>
+    <t>int_rate:12.025-15.74</t>
+  </si>
+  <si>
+    <t>int_rate:15.74-20.281</t>
+  </si>
+  <si>
+    <t>int_rate:&gt;20.281</t>
+  </si>
+  <si>
+    <t>mths_since_earliest_cr_line:&lt;140</t>
+  </si>
+  <si>
+    <t>mths_since_earliest_cr_line:141-164</t>
+  </si>
+  <si>
+    <t>mths_since_earliest_cr_line:165-247</t>
+  </si>
+  <si>
+    <t>mths_since_earliest_cr_line:248-270</t>
+  </si>
+  <si>
+    <t>mths_since_earliest_cr_line:271-352</t>
+  </si>
+  <si>
+    <t>mths_since_earliest_cr_line:&gt;352</t>
+  </si>
+  <si>
+    <t>delinq_2yrs:0</t>
+  </si>
+  <si>
+    <t>delinq_2yrs:1-3</t>
+  </si>
+  <si>
+    <t>delinq_2yrs:&gt;=4</t>
+  </si>
+  <si>
+    <t>inq_last_6mths:0</t>
+  </si>
+  <si>
+    <t>inq_last_6mths:1-2</t>
+  </si>
+  <si>
+    <t>inq_last_6mths:3-6</t>
+  </si>
+  <si>
+    <t>inq_last_6mths:&gt;6</t>
+  </si>
+  <si>
+    <t>open_acc:0</t>
+  </si>
+  <si>
+    <t>open_acc:1-3</t>
+  </si>
+  <si>
+    <t>open_acc:4-12</t>
+  </si>
+  <si>
+    <t>open_acc:13-17</t>
+  </si>
+  <si>
+    <t>open_acc:18-22</t>
+  </si>
+  <si>
+    <t>open_acc:23-25</t>
+  </si>
+  <si>
+    <t>open_acc:26-30</t>
+  </si>
+  <si>
+    <t>open_acc:&gt;=31</t>
+  </si>
+  <si>
+    <t>pub_rec:0-2</t>
+  </si>
+  <si>
+    <t>pub_rec:3-4</t>
+  </si>
+  <si>
+    <t>pub_rec:&gt;=5</t>
+  </si>
+  <si>
+    <t>total_acc:&lt;=27</t>
+  </si>
+  <si>
+    <t>total_acc:28-51</t>
+  </si>
+  <si>
+    <t>total_acc:&gt;=52</t>
+  </si>
+  <si>
+    <t>acc_now_delinq:0</t>
+  </si>
+  <si>
+    <t>acc_now_delinq:&gt;=1</t>
+  </si>
+  <si>
+    <t>total_rev_hi_lim:&lt;=5K</t>
+  </si>
+  <si>
+    <t>total_rev_hi_lim:5K-10K</t>
+  </si>
+  <si>
+    <t>total_rev_hi_lim:10K-20K</t>
+  </si>
+  <si>
+    <t>total_rev_hi_lim:20K-30K</t>
+  </si>
+  <si>
+    <t>total_rev_hi_lim:30K-40K</t>
+  </si>
+  <si>
+    <t>total_rev_hi_lim:40K-55K</t>
+  </si>
+  <si>
+    <t>total_rev_hi_lim:55K-95K</t>
+  </si>
+  <si>
+    <t>total_rev_hi_lim:&gt;95K</t>
+  </si>
+  <si>
+    <t>annual_inc:&lt;20K</t>
+  </si>
+  <si>
+    <t>annual_inc:20K-30K</t>
+  </si>
+  <si>
+    <t>annual_inc:30K-40K</t>
+  </si>
+  <si>
+    <t>annual_inc:40K-50K</t>
+  </si>
+  <si>
+    <t>annual_inc:50K-60K</t>
+  </si>
+  <si>
+    <t>annual_inc:60K-70K</t>
+  </si>
+  <si>
+    <t>annual_inc:70K-80K</t>
+  </si>
+  <si>
+    <t>annual_inc:80K-90K</t>
+  </si>
+  <si>
+    <t>annual_inc:90K-100K</t>
+  </si>
+  <si>
+    <t>annual_inc:100K-120K</t>
+  </si>
+  <si>
+    <t>annual_inc:120K-140K</t>
+  </si>
+  <si>
+    <t>annual_inc:&gt;140K</t>
+  </si>
+  <si>
+    <t>dti:&lt;=1.4</t>
+  </si>
+  <si>
+    <t>dti:1.4-3.5</t>
+  </si>
+  <si>
+    <t>dti:3.5-7.7</t>
+  </si>
+  <si>
+    <t>dti:7.7-10.5</t>
+  </si>
+  <si>
+    <t>dti:10.5-16.1</t>
+  </si>
+  <si>
+    <t>dti:16.1-20.3</t>
+  </si>
+  <si>
+    <t>dti:20.3-21.7</t>
+  </si>
+  <si>
+    <t>dti:21.7-22.4</t>
+  </si>
+  <si>
+    <t>dti:22.4-35</t>
+  </si>
+  <si>
+    <t>dti:&gt;35</t>
+  </si>
+  <si>
+    <t>mths_since_last_delinq:Missing</t>
+  </si>
+  <si>
+    <t>mths_since_last_delinq:0-3</t>
+  </si>
+  <si>
+    <t>mths_since_last_delinq:4-30</t>
+  </si>
+  <si>
+    <t>mths_since_last_delinq:31-56</t>
+  </si>
+  <si>
+    <t>mths_since_last_delinq:&gt;=57</t>
+  </si>
+  <si>
+    <t>mths_since_last_record:Missing</t>
+  </si>
+  <si>
+    <t>mths_since_last_record:0-2</t>
+  </si>
+  <si>
+    <t>mths_since_last_record:3-20</t>
+  </si>
+  <si>
+    <t>mths_since_last_record:21-31</t>
+  </si>
+  <si>
+    <t>mths_since_last_record:32-80</t>
+  </si>
+  <si>
+    <t>mths_since_last_record:81-86</t>
+  </si>
+  <si>
+    <t>mths_since_last_record:&gt;=86</t>
   </si>
 </sst>
 </file>
@@ -410,146 +734,682 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:B127"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="42.28515625" customWidth="1"/>
+    <col min="1" max="1" width="53.28515625" customWidth="1"/>
     <col min="4" max="5" width="31.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="B1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B2">
         <v>0</v>
       </c>
-      <c r="D2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
-      <c r="D3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B4">
         <v>0</v>
       </c>
-      <c r="D4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B5">
         <v>0</v>
       </c>
-      <c r="D5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B6">
         <v>0</v>
       </c>
-      <c r="D6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B7">
         <v>0</v>
       </c>
-      <c r="D7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B8">
         <v>1</v>
       </c>
-      <c r="D8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="B9">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="B10">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="B11">
         <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>127</v>
       </c>
     </row>
   </sheetData>

</xml_diff>